<commit_message>
This is a temporary hack for Heroku UTF8 encoding problem for profile descriptions.
</commit_message>
<xml_diff>
--- a/db/calculations_data.xlsx
+++ b/db/calculations_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="32120" yWindow="-360" windowWidth="32000" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Circles" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="263">
   <si>
     <t>Standard Deviation</t>
   </si>
@@ -617,9 +617,6 @@
   </si>
   <si>
     <t>Agreeableness</t>
-  </si>
-  <si>
-    <t>Conscientousness</t>
   </si>
   <si>
     <t>Mean</t>
@@ -1388,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1414,28 +1411,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>3</v>
@@ -1481,7 +1478,7 @@
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1">
       <c r="A3" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B3" s="2">
         <v>0.8</v>
@@ -1701,7 +1698,7 @@
         <v>29.2</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>193</v>
@@ -1853,7 +1850,7 @@
         <v>30</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>194</v>
@@ -1891,7 +1888,7 @@
         <v>20.3</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>194</v>
@@ -1929,7 +1926,7 @@
         <v>24.1</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>194</v>
@@ -1967,7 +1964,7 @@
         <v>27.5</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>194</v>
@@ -2005,7 +2002,7 @@
         <v>31.5</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>194</v>
@@ -2043,7 +2040,7 @@
         <v>34.1</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>194</v>
@@ -2051,66 +2048,66 @@
     </row>
     <row r="18" spans="1:12" s="3" customFormat="1">
       <c r="A18" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="3" customFormat="1">
       <c r="A20" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="3" customFormat="1">
       <c r="A21" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="3" customFormat="1">
       <c r="A22" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1">
       <c r="A23" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="3" customFormat="1">
       <c r="A24" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="3" customFormat="1">
       <c r="A25" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2135,15 +2132,15 @@
     </row>
     <row r="33" spans="1:7">
       <c r="B33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -2159,7 +2156,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -2175,7 +2172,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B36">
         <v>0.53</v>
@@ -2195,12 +2192,12 @@
     </row>
     <row r="37" spans="1:7">
       <c r="C37" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -2216,7 +2213,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2232,7 +2229,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2273,7 +2270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FT170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2807,7 +2804,7 @@
     </row>
     <row r="2" spans="1:176">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -3328,7 +3325,7 @@
     </row>
     <row r="3" spans="1:176">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3849,7 +3846,7 @@
     </row>
     <row r="4" spans="1:176">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -4370,7 +4367,7 @@
     </row>
     <row r="5" spans="1:176" ht="17.25" customHeight="1">
       <c r="A5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -4891,7 +4888,7 @@
     </row>
     <row r="6" spans="1:176">
       <c r="A6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -5933,7 +5930,7 @@
     </row>
     <row r="9" spans="1:176">
       <c r="A9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C9" s="6">
         <v>12.053941908713693</v>
@@ -6460,7 +6457,7 @@
     <row r="11" spans="1:176">
       <c r="O11" s="6"/>
       <c r="DS11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:176">
@@ -6627,13 +6624,13 @@
     </row>
     <row r="13" spans="1:176">
       <c r="A13" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K13" t="s">
         <v>4</v>
@@ -6654,7 +6651,7 @@
     <row r="14" spans="1:176">
       <c r="A14" s="5"/>
       <c r="I14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J14">
         <v>10</v>
@@ -6682,13 +6679,13 @@
     </row>
     <row r="15" spans="1:176">
       <c r="A15" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J15">
         <v>5</v>
@@ -6716,13 +6713,13 @@
     </row>
     <row r="16" spans="1:176">
       <c r="A16" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J16">
         <v>7</v>
@@ -6750,13 +6747,13 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J17">
         <v>15</v>
@@ -6784,13 +6781,13 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K18">
         <f>SUM(K14:K17)</f>
@@ -6815,7 +6812,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -6843,7 +6840,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -6852,7 +6849,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -6861,7 +6858,7 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -6870,7 +6867,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -6879,7 +6876,7 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -6888,52 +6885,52 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O26" s="8"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B27" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O27" s="8"/>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O28" s="8"/>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O29" s="8"/>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B30">
         <v>7</v>
@@ -6942,7 +6939,7 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B31">
         <v>7</v>
@@ -6951,7 +6948,7 @@
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B32">
         <v>7</v>
@@ -6960,7 +6957,7 @@
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B33">
         <v>7</v>
@@ -6969,7 +6966,7 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B34">
         <v>7</v>

</xml_diff>